<commit_message>
added recoveyr dates to CE01ISSP_00006 and CE02SHSP_00003
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00006.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00006.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaesm/Documents/dev/repos/ooi-integration/asset-management/ARCHIVE/deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="465" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="579"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -26,11 +26,19 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$I$50</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="117">
   <si>
     <t>Ref Des</t>
   </si>
@@ -391,6 +399,9 @@
   </si>
   <si>
     <t>OL000617</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -2268,28 +2279,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>115</v>
       </c>
@@ -2346,7 +2357,9 @@
       <c r="F2" s="31">
         <v>0.96527777777777779</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="32">
+        <v>42645</v>
+      </c>
       <c r="H2" s="48">
         <v>44.662050000000001</v>
       </c>
@@ -2362,91 +2375,91 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:14" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="4:7" s="9" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -2460,29 +2473,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="17" style="34" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2522,7 +2535,7 @@
       <c r="H2" s="47"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>70</v>
       </c>
@@ -2549,7 +2562,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2559,7 +2572,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>71</v>
       </c>
@@ -2617,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="22"/>
@@ -2628,7 +2641,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>72</v>
       </c>
@@ -2657,7 +2670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>72</v>
       </c>
@@ -2677,7 +2690,7 @@
         <v>315</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="H9" s="45">
         <v>-124.09595</v>
@@ -2686,7 +2699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>72</v>
       </c>
@@ -2715,7 +2728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>72</v>
       </c>
@@ -2744,7 +2757,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="22"/>
@@ -2755,7 +2768,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>78</v>
       </c>
@@ -2784,7 +2797,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>78</v>
       </c>
@@ -2813,7 +2826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>78</v>
       </c>
@@ -2842,7 +2855,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>78</v>
       </c>
@@ -2871,7 +2884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>78</v>
       </c>
@@ -2900,7 +2913,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>78</v>
       </c>
@@ -2929,7 +2942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>78</v>
       </c>
@@ -2958,7 +2971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>78</v>
       </c>
@@ -2987,7 +3000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>78</v>
       </c>
@@ -3016,7 +3029,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>78</v>
       </c>
@@ -3045,7 +3058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -3056,7 +3069,7 @@
       <c r="H23" s="39"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>77</v>
       </c>
@@ -3085,7 +3098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>77</v>
       </c>
@@ -3114,7 +3127,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>77</v>
       </c>
@@ -3143,7 +3156,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>77</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
         <v>77</v>
       </c>
@@ -3201,7 +3214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>77</v>
       </c>
@@ -3230,7 +3243,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>77</v>
       </c>
@@ -3259,7 +3272,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="22"/>
@@ -3270,7 +3283,7 @@
       <c r="H31" s="39"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>76</v>
       </c>
@@ -3297,7 +3310,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>76</v>
       </c>
@@ -3324,7 +3337,7 @@
       </c>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>76</v>
       </c>
@@ -3351,7 +3364,7 @@
       </c>
       <c r="I34" s="25"/>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>76</v>
       </c>
@@ -3378,7 +3391,7 @@
       </c>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>76</v>
       </c>
@@ -3405,7 +3418,7 @@
       </c>
       <c r="I36" s="25"/>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>76</v>
       </c>
@@ -3432,7 +3445,7 @@
       </c>
       <c r="I37" s="25"/>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>76</v>
       </c>
@@ -3459,7 +3472,7 @@
       </c>
       <c r="I38" s="25"/>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
@@ -3486,7 +3499,7 @@
       </c>
       <c r="I39" s="25"/>
     </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="22"/>
@@ -3497,7 +3510,7 @@
       <c r="H40" s="39"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>75</v>
       </c>
@@ -3526,7 +3539,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>75</v>
       </c>
@@ -3555,7 +3568,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>75</v>
       </c>
@@ -3582,7 +3595,7 @@
       </c>
       <c r="I43" s="16"/>
     </row>
-    <row r="44" spans="1:9" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A44" s="27"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -3593,7 +3606,7 @@
       <c r="H44" s="41"/>
       <c r="I44" s="27"/>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>74</v>
       </c>
@@ -3620,7 +3633,7 @@
       </c>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
         <v>74</v>
       </c>
@@ -3647,7 +3660,7 @@
       </c>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>74</v>
       </c>
@@ -3674,7 +3687,7 @@
       </c>
       <c r="I47" s="16"/>
     </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="22"/>
@@ -3685,7 +3698,7 @@
       <c r="H48" s="39"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
         <v>73</v>
       </c>
@@ -3714,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
         <v>73</v>
       </c>
@@ -3743,10 +3756,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F51" s="34"/>
     </row>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F52" s="34"/>
     </row>
   </sheetData>
@@ -3764,12 +3777,12 @@
       <selection sqref="A1:AJ83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="16384" width="8.83203125" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="43">
         <v>-3.0190000000000002E-2</v>
       </c>
@@ -3879,7 +3892,7 @@
         <v>1.9692000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="43">
         <v>-2.0278999999999998E-2</v>
       </c>
@@ -3989,7 +4002,7 @@
         <v>1.0718999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="43">
         <v>-1.0749E-2</v>
       </c>
@@ -4099,7 +4112,7 @@
         <v>4.2890000000000003E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="43">
         <v>-2.5699999999999998E-3</v>
       </c>
@@ -4209,7 +4222,7 @@
         <v>-2.9729999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <v>3.4650000000000002E-3</v>
       </c>
@@ -4319,7 +4332,7 @@
         <v>-6.966E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="43">
         <v>8.3379999999999999E-3</v>
       </c>
@@ -4429,7 +4442,7 @@
         <v>-5.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="43">
         <v>1.0692999999999999E-2</v>
       </c>
@@ -4539,7 +4552,7 @@
         <v>-7.7149999999999996E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="43">
         <v>1.179E-2</v>
       </c>
@@ -4649,7 +4662,7 @@
         <v>-6.7790000000000003E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="43">
         <v>1.1067E-2</v>
       </c>
@@ -4759,7 +4772,7 @@
         <v>-5.6220000000000003E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="43">
         <v>1.0867E-2</v>
       </c>
@@ -4869,7 +4882,7 @@
         <v>-5.7860000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="43">
         <v>9.9139999999999992E-3</v>
       </c>
@@ -4979,7 +4992,7 @@
         <v>-4.8609999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="43">
         <v>8.9899999999999997E-3</v>
       </c>
@@ -5089,7 +5102,7 @@
         <v>-3.7429999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="43">
         <v>9.273E-3</v>
       </c>
@@ -5199,7 +5212,7 @@
         <v>-3.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="43">
         <v>8.9759999999999996E-3</v>
       </c>
@@ -5309,7 +5322,7 @@
         <v>-2.627E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="43">
         <v>8.9589999999999999E-3</v>
       </c>
@@ -5419,7 +5432,7 @@
         <v>-2.8530000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="43">
         <v>9.0329999999999994E-3</v>
       </c>
@@ -5529,7 +5542,7 @@
         <v>-2.4060000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="43">
         <v>8.4049999999999993E-3</v>
       </c>
@@ -5639,7 +5652,7 @@
         <v>-1.5969999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="43">
         <v>7.9649999999999999E-3</v>
       </c>
@@ -5749,7 +5762,7 @@
         <v>-1.116E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="43">
         <v>7.2810000000000001E-3</v>
       </c>
@@ -5859,7 +5872,7 @@
         <v>-8.3100000000000003E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="43">
         <v>6.8999999999999999E-3</v>
       </c>
@@ -5969,7 +5982,7 @@
         <v>-6.5300000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>6.5449999999999996E-3</v>
       </c>
@@ -6079,7 +6092,7 @@
         <v>-1.6899999999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="43">
         <v>6.4879999999999998E-3</v>
       </c>
@@ -6189,7 +6202,7 @@
         <v>3.1000000000000001E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="43">
         <v>6.2290000000000002E-3</v>
       </c>
@@ -6299,7 +6312,7 @@
         <v>5.1099999999999995E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="43">
         <v>5.9959999999999996E-3</v>
       </c>
@@ -6409,7 +6422,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="43">
         <v>5.705E-3</v>
       </c>
@@ -6519,7 +6532,7 @@
         <v>6.8800000000000003E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" s="43">
         <v>5.3350000000000003E-3</v>
       </c>
@@ -6629,7 +6642,7 @@
         <v>8.4900000000000004E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="43">
         <v>5.228E-3</v>
       </c>
@@ -6739,7 +6752,7 @@
         <v>1.098E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="43">
         <v>5.0470000000000003E-3</v>
       </c>
@@ -6849,7 +6862,7 @@
         <v>1.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="43">
         <v>4.921E-3</v>
       </c>
@@ -6959,7 +6972,7 @@
         <v>1.286E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="43">
         <v>4.7660000000000003E-3</v>
       </c>
@@ -7069,7 +7082,7 @@
         <v>1.645E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="43">
         <v>4.6629999999999996E-3</v>
       </c>
@@ -7179,7 +7192,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="43">
         <v>4.3290000000000004E-3</v>
       </c>
@@ -7289,7 +7302,7 @@
         <v>1.7179999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="43">
         <v>4.3899999999999998E-3</v>
       </c>
@@ -7399,7 +7412,7 @@
         <v>1.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="43">
         <v>4.3790000000000001E-3</v>
       </c>
@@ -7509,7 +7522,7 @@
         <v>1.8209999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" s="43">
         <v>4.5589999999999997E-3</v>
       </c>
@@ -7619,7 +7632,7 @@
         <v>1.8370000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" s="43">
         <v>4.0619999999999996E-3</v>
       </c>
@@ -7729,7 +7742,7 @@
         <v>1.6980000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37" s="43">
         <v>3.4069999999999999E-3</v>
       </c>
@@ -7839,7 +7852,7 @@
         <v>1.7030000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38" s="43">
         <v>2.7409999999999999E-3</v>
       </c>
@@ -7949,7 +7962,7 @@
         <v>1.5809999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" s="43">
         <v>2.555E-3</v>
       </c>
@@ -8059,7 +8072,7 @@
         <v>1.353E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
         <v>2.5469999999999998E-3</v>
       </c>
@@ -8169,7 +8182,7 @@
         <v>1.3829999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" s="43">
         <v>2.7910000000000001E-3</v>
       </c>
@@ -8279,7 +8292,7 @@
         <v>1.108E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" s="43">
         <v>4.5069999999999997E-3</v>
       </c>
@@ -8389,7 +8402,7 @@
         <v>5.1999999999999997E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" s="43">
         <v>4.646E-3</v>
       </c>
@@ -8499,7 +8512,7 @@
         <v>9.2E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="43">
         <v>4.6740000000000002E-3</v>
       </c>
@@ -8609,7 +8622,7 @@
         <v>-2.5999999999999998E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="43">
         <v>4.5820000000000001E-3</v>
       </c>
@@ -8719,7 +8732,7 @@
         <v>-1.37E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="43">
         <v>4.542E-3</v>
       </c>
@@ -8829,7 +8842,7 @@
         <v>-2.2800000000000001E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" s="43">
         <v>4.5880000000000001E-3</v>
       </c>
@@ -8939,7 +8952,7 @@
         <v>-2.0900000000000001E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="43">
         <v>4.3959999999999997E-3</v>
       </c>
@@ -9049,7 +9062,7 @@
         <v>-2.22E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" s="43">
         <v>4.1989999999999996E-3</v>
       </c>
@@ -9159,7 +9172,7 @@
         <v>-1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" s="43">
         <v>4.1110000000000001E-3</v>
       </c>
@@ -9269,7 +9282,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51" s="43">
         <v>3.9249999999999997E-3</v>
       </c>
@@ -9379,7 +9392,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" s="43">
         <v>3.542E-3</v>
       </c>
@@ -9489,7 +9502,7 @@
         <v>2.52E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="43">
         <v>3.2569999999999999E-3</v>
       </c>
@@ -9599,7 +9612,7 @@
         <v>4.06E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54" s="43">
         <v>3.0820000000000001E-3</v>
       </c>
@@ -9709,7 +9722,7 @@
         <v>4.2499999999999998E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" s="43">
         <v>3.0739999999999999E-3</v>
       </c>
@@ -9819,7 +9832,7 @@
         <v>5.8699999999999996E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" s="43">
         <v>3.0929999999999998E-3</v>
       </c>
@@ -9929,7 +9942,7 @@
         <v>7.2599999999999997E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" s="43">
         <v>3.0850000000000001E-3</v>
       </c>
@@ -10039,7 +10052,7 @@
         <v>8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" s="43">
         <v>3.078E-3</v>
       </c>
@@ -10149,7 +10162,7 @@
         <v>9.3999999999999997E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" s="43">
         <v>3.1480000000000002E-3</v>
       </c>
@@ -10259,7 +10272,7 @@
         <v>1.0790000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60" s="43">
         <v>3.1960000000000001E-3</v>
       </c>
@@ -10369,7 +10382,7 @@
         <v>1.2539999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61" s="43">
         <v>3.3509999999999998E-3</v>
       </c>
@@ -10479,7 +10492,7 @@
         <v>1.2329999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62" s="43">
         <v>3.555E-3</v>
       </c>
@@ -10589,7 +10602,7 @@
         <v>1.2260000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63" s="43">
         <v>3.5400000000000002E-3</v>
       </c>
@@ -10699,7 +10712,7 @@
         <v>1.1709999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A64" s="43">
         <v>3.3999999999999998E-3</v>
       </c>
@@ -10809,7 +10822,7 @@
         <v>1.33E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65" s="43">
         <v>3.431E-3</v>
       </c>
@@ -10919,7 +10932,7 @@
         <v>1.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66" s="43">
         <v>3.2820000000000002E-3</v>
       </c>
@@ -11029,7 +11042,7 @@
         <v>1.474E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67" s="43">
         <v>3.0709999999999999E-3</v>
       </c>
@@ -11139,7 +11152,7 @@
         <v>1.3669999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68" s="43">
         <v>2.7039999999999998E-3</v>
       </c>
@@ -11249,7 +11262,7 @@
         <v>1.3550000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69" s="43">
         <v>1.892E-3</v>
       </c>
@@ -11359,7 +11372,7 @@
         <v>1.441E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70" s="43">
         <v>1.3780000000000001E-3</v>
       </c>
@@ -11469,7 +11482,7 @@
         <v>1.449E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71" s="43">
         <v>9.5600000000000004E-4</v>
       </c>
@@ -11579,7 +11592,7 @@
         <v>1.4270000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72" s="43">
         <v>6.4499999999999996E-4</v>
       </c>
@@ -11689,7 +11702,7 @@
         <v>1.598E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73" s="43">
         <v>3.4600000000000001E-4</v>
       </c>
@@ -11799,7 +11812,7 @@
         <v>1.745E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74" s="43">
         <v>3.0000000000000001E-6</v>
       </c>
@@ -11909,7 +11922,7 @@
         <v>1.7899999999999999E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75" s="43">
         <v>-7.7000000000000001E-5</v>
       </c>
@@ -12019,7 +12032,7 @@
         <v>1.9469999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76" s="43">
         <v>8.3999999999999995E-5</v>
       </c>
@@ -12129,7 +12142,7 @@
         <v>2.0100000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77" s="43">
         <v>-1.1E-4</v>
       </c>
@@ -12239,7 +12252,7 @@
         <v>1.967E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78" s="43">
         <v>-1.4799999999999999E-4</v>
       </c>
@@ -12349,7 +12362,7 @@
         <v>1.905E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79" s="43">
         <v>-8.8999999999999995E-5</v>
       </c>
@@ -12459,7 +12472,7 @@
         <v>1.8810000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80" s="43">
         <v>3.2499999999999999E-4</v>
       </c>
@@ -12569,7 +12582,7 @@
         <v>1.897E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81" s="43">
         <v>2.7700000000000001E-4</v>
       </c>
@@ -12679,7 +12692,7 @@
         <v>1.6800000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" s="43">
         <v>7.8399999999999997E-4</v>
       </c>
@@ -12789,7 +12802,7 @@
         <v>1.449E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83" s="43">
         <v>7.45E-4</v>
       </c>
@@ -12912,12 +12925,12 @@
       <selection sqref="A1:AJ83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="16384" width="8.83203125" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="43">
         <v>-3.6998999999999997E-2</v>
       </c>
@@ -13027,7 +13040,7 @@
         <v>-7.2420000000000002E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="43">
         <v>-3.1243E-2</v>
       </c>
@@ -13137,7 +13150,7 @@
         <v>-1.418E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="43">
         <v>-3.0123E-2</v>
       </c>
@@ -13247,7 +13260,7 @@
         <v>-4.3150000000000003E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="43">
         <v>-2.6842999999999999E-2</v>
       </c>
@@ -13357,7 +13370,7 @@
         <v>-1.707E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <v>-2.1867999999999999E-2</v>
       </c>
@@ -13467,7 +13480,7 @@
         <v>-3.4350000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="43">
         <v>-2.0025000000000001E-2</v>
       </c>
@@ -13577,7 +13590,7 @@
         <v>-1.567E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="43">
         <v>-1.8008E-2</v>
       </c>
@@ -13687,7 +13700,7 @@
         <v>-5.1580000000000003E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="43">
         <v>-1.7402000000000001E-2</v>
       </c>
@@ -13797,7 +13810,7 @@
         <v>-4.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="43">
         <v>-1.7918E-2</v>
       </c>
@@ -13907,7 +13920,7 @@
         <v>-2.6649999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="43">
         <v>-1.7467E-2</v>
       </c>
@@ -14017,7 +14030,7 @@
         <v>-4.3249999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="43">
         <v>-1.7302000000000001E-2</v>
       </c>
@@ -14127,7 +14140,7 @@
         <v>-1.6169999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="43">
         <v>-1.7683999999999998E-2</v>
       </c>
@@ -14237,7 +14250,7 @@
         <v>-1.34E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="43">
         <v>-1.9014E-2</v>
       </c>
@@ -14347,7 +14360,7 @@
         <v>-1.9070000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="43">
         <v>-1.7864000000000001E-2</v>
       </c>
@@ -14457,7 +14470,7 @@
         <v>-3.4999999999999997E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="43">
         <v>-1.7988000000000001E-2</v>
       </c>
@@ -14567,7 +14580,7 @@
         <v>-1.3100000000000001E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="43">
         <v>-1.8012E-2</v>
       </c>
@@ -14677,7 +14690,7 @@
         <v>8.1300000000000003E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="43">
         <v>-1.7312000000000001E-2</v>
       </c>
@@ -14787,7 +14800,7 @@
         <v>1.5699999999999999E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="43">
         <v>-1.6289999999999999E-2</v>
       </c>
@@ -14897,7 +14910,7 @@
         <v>-8.2000000000000001E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="43">
         <v>-1.5969000000000001E-2</v>
       </c>
@@ -15007,7 +15020,7 @@
         <v>-4.4900000000000002E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="43">
         <v>-1.3956E-2</v>
       </c>
@@ -15117,7 +15130,7 @@
         <v>1.1400000000000001E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>-1.2460000000000001E-2</v>
       </c>
@@ -15227,7 +15240,7 @@
         <v>-1.7960000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="43">
         <v>-1.291E-2</v>
       </c>
@@ -15337,7 +15350,7 @@
         <v>-1.1670000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="43">
         <v>-1.1282E-2</v>
       </c>
@@ -15447,7 +15460,7 @@
         <v>-1.6459999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="43">
         <v>-1.1135000000000001E-2</v>
       </c>
@@ -15557,7 +15570,7 @@
         <v>-2.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="43">
         <v>-1.1556E-2</v>
       </c>
@@ -15667,7 +15680,7 @@
         <v>-1.913E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" s="43">
         <v>-1.1502E-2</v>
       </c>
@@ -15777,7 +15790,7 @@
         <v>-1.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="43">
         <v>-1.2137E-2</v>
       </c>
@@ -15887,7 +15900,7 @@
         <v>-1.439E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="43">
         <v>-1.2751E-2</v>
       </c>
@@ -15997,7 +16010,7 @@
         <v>-5.4500000000000002E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="43">
         <v>-1.3379E-2</v>
       </c>
@@ -16107,7 +16120,7 @@
         <v>-4.3600000000000003E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="43">
         <v>-1.4312E-2</v>
       </c>
@@ -16217,7 +16230,7 @@
         <v>-2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="43">
         <v>-1.4709E-2</v>
       </c>
@@ -16327,7 +16340,7 @@
         <v>6.8999999999999997E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="43">
         <v>-1.5193999999999999E-2</v>
       </c>
@@ -16437,7 +16450,7 @@
         <v>8.9499999999999996E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="43">
         <v>-1.5633999999999999E-2</v>
       </c>
@@ -16547,7 +16560,7 @@
         <v>1.4430000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="43">
         <v>-1.5495999999999999E-2</v>
       </c>
@@ -16657,7 +16670,7 @@
         <v>1.4430000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" s="43">
         <v>-1.5431E-2</v>
       </c>
@@ -16767,7 +16780,7 @@
         <v>1.472E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" s="43">
         <v>-1.4796E-2</v>
       </c>
@@ -16877,7 +16890,7 @@
         <v>1.48E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37" s="43">
         <v>-1.4559000000000001E-2</v>
       </c>
@@ -16987,7 +17000,7 @@
         <v>1.31E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38" s="43">
         <v>-1.4137E-2</v>
       </c>
@@ -17097,7 +17110,7 @@
         <v>5.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" s="43">
         <v>-1.3273999999999999E-2</v>
       </c>
@@ -17207,7 +17220,7 @@
         <v>6.8400000000000004E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
         <v>-1.1788E-2</v>
       </c>
@@ -17317,7 +17330,7 @@
         <v>-1.55E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" s="43">
         <v>-1.0460000000000001E-2</v>
       </c>
@@ -17427,7 +17440,7 @@
         <v>-5.6700000000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" s="43">
         <v>-5.8589999999999996E-3</v>
       </c>
@@ -17537,7 +17550,7 @@
         <v>-1.735E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" s="43">
         <v>-4.1939999999999998E-3</v>
       </c>
@@ -17647,7 +17660,7 @@
         <v>-2.317E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="43">
         <v>-3.2810000000000001E-3</v>
       </c>
@@ -17757,7 +17770,7 @@
         <v>-2.5240000000000002E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="43">
         <v>-1.936E-3</v>
       </c>
@@ -17867,7 +17880,7 @@
         <v>-2.9260000000000002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="43">
         <v>-6.1799999999999995E-4</v>
       </c>
@@ -17977,7 +17990,7 @@
         <v>-3.0950000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" s="43">
         <v>-1.8000000000000001E-4</v>
       </c>
@@ -18087,7 +18100,7 @@
         <v>-3.5019999999999999E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="43">
         <v>5.4600000000000004E-4</v>
       </c>
@@ -18197,7 +18210,7 @@
         <v>-3.784E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" s="43">
         <v>1.1800000000000001E-3</v>
       </c>
@@ -18307,7 +18320,7 @@
         <v>-3.9259999999999998E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" s="43">
         <v>1.1299999999999999E-3</v>
       </c>
@@ -18417,7 +18430,7 @@
         <v>-3.725E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51" s="43">
         <v>1.2459999999999999E-3</v>
       </c>
@@ -18527,7 +18540,7 @@
         <v>-3.715E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" s="43">
         <v>6.5600000000000001E-4</v>
       </c>
@@ -18637,7 +18650,7 @@
         <v>-3.6830000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="43">
         <v>5.3700000000000004E-4</v>
       </c>
@@ -18747,7 +18760,7 @@
         <v>-3.4009999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54" s="43">
         <v>-6.2000000000000003E-5</v>
       </c>
@@ -18857,7 +18870,7 @@
         <v>-3.0149999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" s="43">
         <v>-1.06E-3</v>
       </c>
@@ -18967,7 +18980,7 @@
         <v>-2.7529999999999998E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" s="43">
         <v>-1.572E-3</v>
       </c>
@@ -19077,7 +19090,7 @@
         <v>-2.3900000000000002E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" s="43">
         <v>-2.166E-3</v>
       </c>
@@ -19187,7 +19200,7 @@
         <v>-1.98E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" s="43">
         <v>-3.2850000000000002E-3</v>
       </c>
@@ -19297,7 +19310,7 @@
         <v>-1.781E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" s="43">
         <v>-3.82E-3</v>
       </c>
@@ -19407,7 +19420,7 @@
         <v>-1.3339999999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60" s="43">
         <v>-4.2059999999999997E-3</v>
       </c>
@@ -19517,7 +19530,7 @@
         <v>-1.103E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61" s="43">
         <v>-4.9820000000000003E-3</v>
       </c>
@@ -19627,7 +19640,7 @@
         <v>-9.1399999999999999E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62" s="43">
         <v>-5.1390000000000003E-3</v>
       </c>
@@ -19737,7 +19750,7 @@
         <v>-5.3200000000000003E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63" s="43">
         <v>-5.365E-3</v>
       </c>
@@ -19847,7 +19860,7 @@
         <v>-3.68E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A64" s="43">
         <v>-5.7980000000000002E-3</v>
       </c>
@@ -19957,7 +19970,7 @@
         <v>-2.9100000000000003E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65" s="43">
         <v>-5.7369999999999999E-3</v>
       </c>
@@ -20067,7 +20080,7 @@
         <v>-8.0000000000000007E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66" s="43">
         <v>-6.0089999999999996E-3</v>
       </c>
@@ -20177,7 +20190,7 @@
         <v>-1.11E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67" s="43">
         <v>-6.6740000000000002E-3</v>
       </c>
@@ -20287,7 +20300,7 @@
         <v>-4.0299999999999998E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68" s="43">
         <v>-6.2979999999999998E-3</v>
       </c>
@@ -20397,7 +20410,7 @@
         <v>-2.2100000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69" s="43">
         <v>-6.8129999999999996E-3</v>
       </c>
@@ -20507,7 +20520,7 @@
         <v>-3.59E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70" s="43">
         <v>-6.6290000000000003E-3</v>
       </c>
@@ -20617,7 +20630,7 @@
         <v>-7.7899999999999996E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71" s="43">
         <v>-5.8869999999999999E-3</v>
       </c>
@@ -20727,7 +20740,7 @@
         <v>-5.13E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72" s="43">
         <v>-5.4780000000000002E-3</v>
       </c>
@@ -20837,7 +20850,7 @@
         <v>-8.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73" s="43">
         <v>-4.888E-3</v>
       </c>
@@ -20947,7 +20960,7 @@
         <v>-9.5699999999999995E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74" s="43">
         <v>-3.8509999999999998E-3</v>
       </c>
@@ -21057,7 +21070,7 @@
         <v>-8.3699999999999996E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75" s="43">
         <v>-4.2779999999999997E-3</v>
       </c>
@@ -21167,7 +21180,7 @@
         <v>-1.67E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76" s="43">
         <v>-3.408E-3</v>
       </c>
@@ -21277,7 +21290,7 @@
         <v>-1.39E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77" s="43">
         <v>-3.3180000000000002E-3</v>
       </c>
@@ -21387,7 +21400,7 @@
         <v>-1.6720000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78" s="43">
         <v>-1.5969999999999999E-3</v>
       </c>
@@ -21497,7 +21510,7 @@
         <v>-1.6850000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79" s="43">
         <v>-3.0400000000000002E-3</v>
       </c>
@@ -21607,7 +21620,7 @@
         <v>-2.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80" s="43">
         <v>-1.5839999999999999E-3</v>
       </c>
@@ -21717,7 +21730,7 @@
         <v>-1.967E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81" s="43">
         <v>-1.286E-3</v>
       </c>
@@ -21827,7 +21840,7 @@
         <v>-2.4689999999999998E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" s="43">
         <v>-1.6000000000000001E-4</v>
       </c>
@@ -21937,7 +21950,7 @@
         <v>-3.016E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83" s="43">
         <v>-1.0900000000000001E-4</v>
       </c>

</xml_diff>